<commit_message>
best maching event and comments
</commit_message>
<xml_diff>
--- a/input/AnalyticsSheets/StoreLocator.xlsx
+++ b/input/AnalyticsSheets/StoreLocator.xlsx
@@ -22,9 +22,6 @@
     <t>Expected values</t>
   </si>
   <si>
-    <t>event</t>
-  </si>
-  <si>
     <t>Storelocator</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>Store Locator Options - ${productName}</t>
+  </si>
+  <si>
+    <t>event1</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,19 +687,19 @@
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -707,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -725,19 +725,19 @@
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -745,16 +745,16 @@
         <v>0</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -762,16 +762,16 @@
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -779,13 +779,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>